<commit_message>
Commit Test on new Desktop
</commit_message>
<xml_diff>
--- a/SimpleProjects/Module/ParkingArea/1.Design/Database/Database_Specification.xlsx
+++ b/SimpleProjects/Module/ParkingArea/1.Design/Database/Database_Specification.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr codeName="현재_통합_문서"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kururu_Folder\Kururu_Programming\Repositories\1.Documents\Kururu_Documents\SimpleProjects\Module\ParkingArea\1.Design\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kururu_Develop\Kururu_Programming\Repositories\1.Documents\Kururu_Documents\SimpleProjects\Module\ParkingArea\1.Design\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E83F25-D40D-4155-BE67-D041F7EF46F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14955" windowHeight="7560"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database_Sheet" sheetId="1" r:id="rId1"/>
@@ -21,10 +22,16 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">ENTRY_BOOK!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">LOT_INFORMATION!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -275,7 +282,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="13"/>
@@ -757,109 +764,109 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -921,7 +928,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Task List" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Task List" pivot="0" count="4">
+    <tableStyle name="Task List" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="3"/>
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="totalRow" dxfId="1"/>
@@ -956,7 +963,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="그림 6"/>
+        <xdr:cNvPr id="7" name="그림 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -994,7 +1007,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1222,7 +1241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -1737,7 +1756,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T9:V14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T9:V14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"○,"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1752,7 +1771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -1780,38 +1799,38 @@
       <c r="F1" s="22"/>
     </row>
     <row r="2" spans="2:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
       <c r="R2" s="8"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="43" t="s">
+      <c r="T2" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="43"/>
-      <c r="AF2" s="43"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="74"/>
+      <c r="AA2" s="74"/>
+      <c r="AB2" s="74"/>
+      <c r="AC2" s="74"/>
+      <c r="AD2" s="74"/>
+      <c r="AE2" s="74"/>
+      <c r="AF2" s="74"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
@@ -1821,38 +1840,38 @@
       <c r="AM2" s="6"/>
     </row>
     <row r="3" spans="2:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="75"/>
       <c r="R3" s="9"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="44" t="s">
+      <c r="T3" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
-      <c r="W3" s="44"/>
-      <c r="X3" s="44"/>
-      <c r="Y3" s="44"/>
-      <c r="Z3" s="44"/>
-      <c r="AA3" s="44"/>
-      <c r="AB3" s="44"/>
-      <c r="AC3" s="44"/>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
+      <c r="U3" s="75"/>
+      <c r="V3" s="75"/>
+      <c r="W3" s="75"/>
+      <c r="X3" s="75"/>
+      <c r="Y3" s="75"/>
+      <c r="Z3" s="75"/>
+      <c r="AA3" s="75"/>
+      <c r="AB3" s="75"/>
+      <c r="AC3" s="75"/>
+      <c r="AD3" s="75"/>
+      <c r="AE3" s="75"/>
+      <c r="AF3" s="75"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
@@ -1861,36 +1880,36 @@
       <c r="AL3" s="1"/>
     </row>
     <row r="4" spans="2:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="43"/>
-      <c r="AE4" s="43"/>
-      <c r="AF4" s="43"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="74"/>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="74"/>
+      <c r="AE4" s="74"/>
+      <c r="AF4" s="74"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
@@ -1900,36 +1919,36 @@
       <c r="AM4" s="6"/>
     </row>
     <row r="5" spans="2:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="47"/>
-      <c r="U5" s="47"/>
-      <c r="V5" s="47"/>
-      <c r="W5" s="47"/>
-      <c r="X5" s="47"/>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="47"/>
-      <c r="AA5" s="47"/>
-      <c r="AB5" s="47"/>
-      <c r="AC5" s="47"/>
-      <c r="AD5" s="47"/>
-      <c r="AE5" s="47"/>
-      <c r="AF5" s="47"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="65"/>
+      <c r="Z5" s="65"/>
+      <c r="AA5" s="65"/>
+      <c r="AB5" s="65"/>
+      <c r="AC5" s="65"/>
+      <c r="AD5" s="65"/>
+      <c r="AE5" s="65"/>
+      <c r="AF5" s="65"/>
       <c r="AG5" s="7"/>
       <c r="AH5" s="7"/>
       <c r="AI5" s="7"/>
@@ -1953,21 +1972,21 @@
       <c r="O6" s="17"/>
     </row>
     <row r="7" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
       <c r="P7" s="26"/>
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
@@ -1995,58 +2014,58 @@
       <c r="AN7" s="3"/>
     </row>
     <row r="8" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52" t="s">
+      <c r="C8" s="69"/>
+      <c r="D8" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="53" t="s">
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="54" t="s">
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54" t="s">
+      <c r="O8" s="72"/>
+      <c r="P8" s="72"/>
+      <c r="Q8" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="R8" s="54"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54" t="s">
+      <c r="R8" s="72"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="U8" s="54"/>
-      <c r="V8" s="54"/>
-      <c r="W8" s="54" t="s">
+      <c r="U8" s="72"/>
+      <c r="V8" s="72"/>
+      <c r="W8" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="X8" s="54"/>
-      <c r="Y8" s="54"/>
-      <c r="Z8" s="54"/>
-      <c r="AA8" s="54" t="s">
+      <c r="X8" s="72"/>
+      <c r="Y8" s="72"/>
+      <c r="Z8" s="72"/>
+      <c r="AA8" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="AB8" s="54"/>
-      <c r="AC8" s="54"/>
-      <c r="AD8" s="54"/>
-      <c r="AE8" s="54"/>
-      <c r="AF8" s="54" t="s">
+      <c r="AB8" s="72"/>
+      <c r="AC8" s="72"/>
+      <c r="AD8" s="72"/>
+      <c r="AE8" s="72"/>
+      <c r="AF8" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="AG8" s="54"/>
-      <c r="AH8" s="54"/>
-      <c r="AI8" s="55"/>
+      <c r="AG8" s="72"/>
+      <c r="AH8" s="72"/>
+      <c r="AI8" s="73"/>
       <c r="AJ8" s="27"/>
       <c r="AK8" s="4"/>
       <c r="AL8" s="4"/>
@@ -2054,57 +2073,57 @@
       <c r="AN8" s="4"/>
     </row>
     <row r="9" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="59">
+      <c r="B9" s="45">
         <f>ROW()-8</f>
         <v>1</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="61" t="s">
+      <c r="C9" s="46"/>
+      <c r="D9" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="65" t="s">
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="45" t="s">
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="O9" s="45"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="46" t="s">
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="56" t="s">
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="U9" s="56"/>
-      <c r="V9" s="57"/>
-      <c r="W9" s="57" t="s">
+      <c r="U9" s="49"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="X9" s="57"/>
-      <c r="Y9" s="57"/>
-      <c r="Z9" s="57"/>
-      <c r="AA9" s="57"/>
-      <c r="AB9" s="57"/>
-      <c r="AC9" s="57"/>
-      <c r="AD9" s="57"/>
-      <c r="AE9" s="57"/>
-      <c r="AF9" s="57" t="s">
+      <c r="X9" s="43"/>
+      <c r="Y9" s="43"/>
+      <c r="Z9" s="43"/>
+      <c r="AA9" s="43"/>
+      <c r="AB9" s="43"/>
+      <c r="AC9" s="43"/>
+      <c r="AD9" s="43"/>
+      <c r="AE9" s="43"/>
+      <c r="AF9" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="AG9" s="57"/>
-      <c r="AH9" s="57"/>
-      <c r="AI9" s="58"/>
+      <c r="AG9" s="43"/>
+      <c r="AH9" s="43"/>
+      <c r="AI9" s="44"/>
       <c r="AJ9" s="28"/>
       <c r="AK9" s="5"/>
       <c r="AL9" s="5"/>
@@ -2112,53 +2131,53 @@
       <c r="AN9" s="5"/>
     </row>
     <row r="10" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="59">
+      <c r="B10" s="45">
         <f>ROW()-8</f>
         <v>2</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61" t="s">
+      <c r="C10" s="46"/>
+      <c r="D10" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="65" t="s">
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
-      <c r="N10" s="45" t="s">
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="46">
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="48">
         <v>100</v>
       </c>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="56" t="s">
+      <c r="R10" s="48"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="U10" s="56"/>
-      <c r="V10" s="57"/>
-      <c r="W10" s="57"/>
-      <c r="X10" s="57"/>
-      <c r="Y10" s="57"/>
-      <c r="Z10" s="57"/>
-      <c r="AA10" s="57"/>
-      <c r="AB10" s="57"/>
-      <c r="AC10" s="57"/>
-      <c r="AD10" s="57"/>
-      <c r="AE10" s="57"/>
-      <c r="AF10" s="57"/>
-      <c r="AG10" s="57"/>
-      <c r="AH10" s="57"/>
-      <c r="AI10" s="58"/>
+      <c r="U10" s="49"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="43"/>
+      <c r="X10" s="43"/>
+      <c r="Y10" s="43"/>
+      <c r="Z10" s="43"/>
+      <c r="AA10" s="43"/>
+      <c r="AB10" s="43"/>
+      <c r="AC10" s="43"/>
+      <c r="AD10" s="43"/>
+      <c r="AE10" s="43"/>
+      <c r="AF10" s="43"/>
+      <c r="AG10" s="43"/>
+      <c r="AH10" s="43"/>
+      <c r="AI10" s="44"/>
       <c r="AJ10" s="28"/>
       <c r="AK10" s="5"/>
       <c r="AL10" s="5"/>
@@ -2166,17 +2185,17 @@
       <c r="AN10" s="5"/>
     </row>
     <row r="11" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="59">
+      <c r="B11" s="45">
         <f t="shared" ref="B11:B15" si="0">ROW()-8</f>
         <v>3</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61" t="s">
+      <c r="C11" s="46"/>
+      <c r="D11" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
       <c r="H11" s="62" t="s">
         <v>17</v>
       </c>
@@ -2185,34 +2204,34 @@
       <c r="K11" s="63"/>
       <c r="L11" s="63"/>
       <c r="M11" s="64"/>
-      <c r="N11" s="45" t="s">
+      <c r="N11" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="O11" s="45"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="46">
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="48">
         <v>100</v>
       </c>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="57" t="s">
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="U11" s="57"/>
-      <c r="V11" s="57"/>
-      <c r="W11" s="57"/>
-      <c r="X11" s="57"/>
-      <c r="Y11" s="57"/>
-      <c r="Z11" s="57"/>
-      <c r="AA11" s="57"/>
-      <c r="AB11" s="57"/>
-      <c r="AC11" s="57"/>
-      <c r="AD11" s="57"/>
-      <c r="AE11" s="57"/>
-      <c r="AF11" s="57"/>
-      <c r="AG11" s="57"/>
-      <c r="AH11" s="57"/>
-      <c r="AI11" s="58"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="43"/>
+      <c r="X11" s="43"/>
+      <c r="Y11" s="43"/>
+      <c r="Z11" s="43"/>
+      <c r="AA11" s="43"/>
+      <c r="AB11" s="43"/>
+      <c r="AC11" s="43"/>
+      <c r="AD11" s="43"/>
+      <c r="AE11" s="43"/>
+      <c r="AF11" s="43"/>
+      <c r="AG11" s="43"/>
+      <c r="AH11" s="43"/>
+      <c r="AI11" s="44"/>
       <c r="AJ11" s="28"/>
       <c r="AK11" s="5"/>
       <c r="AL11" s="5"/>
@@ -2220,17 +2239,17 @@
       <c r="AN11" s="5"/>
     </row>
     <row r="12" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="59">
+      <c r="B12" s="45">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="61" t="s">
+      <c r="C12" s="46"/>
+      <c r="D12" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="62" t="s">
         <v>30</v>
       </c>
@@ -2239,34 +2258,34 @@
       <c r="K12" s="63"/>
       <c r="L12" s="63"/>
       <c r="M12" s="64"/>
-      <c r="N12" s="45" t="s">
+      <c r="N12" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="46">
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="48">
         <v>100</v>
       </c>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="57" t="s">
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="U12" s="57"/>
-      <c r="V12" s="57"/>
-      <c r="W12" s="57"/>
-      <c r="X12" s="57"/>
-      <c r="Y12" s="57"/>
-      <c r="Z12" s="57"/>
-      <c r="AA12" s="57"/>
-      <c r="AB12" s="57"/>
-      <c r="AC12" s="57"/>
-      <c r="AD12" s="57"/>
-      <c r="AE12" s="57"/>
-      <c r="AF12" s="57"/>
-      <c r="AG12" s="57"/>
-      <c r="AH12" s="57"/>
-      <c r="AI12" s="58"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43"/>
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="43"/>
+      <c r="AD12" s="43"/>
+      <c r="AE12" s="43"/>
+      <c r="AF12" s="43"/>
+      <c r="AG12" s="43"/>
+      <c r="AH12" s="43"/>
+      <c r="AI12" s="44"/>
       <c r="AJ12" s="28"/>
       <c r="AK12" s="5"/>
       <c r="AL12" s="5"/>
@@ -2274,17 +2293,17 @@
       <c r="AN12" s="5"/>
     </row>
     <row r="13" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="59">
+      <c r="B13" s="45">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="61" t="s">
+      <c r="C13" s="46"/>
+      <c r="D13" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
       <c r="H13" s="62" t="s">
         <v>31</v>
       </c>
@@ -2293,34 +2312,34 @@
       <c r="K13" s="63"/>
       <c r="L13" s="63"/>
       <c r="M13" s="64"/>
-      <c r="N13" s="45" t="s">
+      <c r="N13" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="46">
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="48">
         <v>100</v>
       </c>
-      <c r="R13" s="46"/>
-      <c r="S13" s="46"/>
-      <c r="T13" s="57" t="s">
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="U13" s="57"/>
-      <c r="V13" s="57"/>
-      <c r="W13" s="57"/>
-      <c r="X13" s="57"/>
-      <c r="Y13" s="57"/>
-      <c r="Z13" s="57"/>
-      <c r="AA13" s="57"/>
-      <c r="AB13" s="57"/>
-      <c r="AC13" s="57"/>
-      <c r="AD13" s="57"/>
-      <c r="AE13" s="57"/>
-      <c r="AF13" s="57"/>
-      <c r="AG13" s="57"/>
-      <c r="AH13" s="57"/>
-      <c r="AI13" s="58"/>
+      <c r="U13" s="43"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="43"/>
+      <c r="X13" s="43"/>
+      <c r="Y13" s="43"/>
+      <c r="Z13" s="43"/>
+      <c r="AA13" s="43"/>
+      <c r="AB13" s="43"/>
+      <c r="AC13" s="43"/>
+      <c r="AD13" s="43"/>
+      <c r="AE13" s="43"/>
+      <c r="AF13" s="43"/>
+      <c r="AG13" s="43"/>
+      <c r="AH13" s="43"/>
+      <c r="AI13" s="44"/>
       <c r="AJ13" s="28"/>
       <c r="AK13" s="5"/>
       <c r="AL13" s="5"/>
@@ -2328,55 +2347,55 @@
       <c r="AN13" s="5"/>
     </row>
     <row r="14" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="59">
+      <c r="B14" s="45">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="61" t="s">
+      <c r="C14" s="46"/>
+      <c r="D14" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="65" t="s">
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="45" t="s">
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="O14" s="45"/>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="46">
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="48">
         <v>1</v>
       </c>
-      <c r="R14" s="46"/>
-      <c r="S14" s="46"/>
-      <c r="T14" s="57" t="s">
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="U14" s="57"/>
-      <c r="V14" s="57"/>
-      <c r="W14" s="57"/>
-      <c r="X14" s="57"/>
-      <c r="Y14" s="57"/>
-      <c r="Z14" s="57"/>
-      <c r="AA14" s="57"/>
-      <c r="AB14" s="57"/>
-      <c r="AC14" s="57"/>
-      <c r="AD14" s="57"/>
-      <c r="AE14" s="57"/>
-      <c r="AF14" s="56" t="s">
+      <c r="U14" s="43"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="43"/>
+      <c r="Y14" s="43"/>
+      <c r="Z14" s="43"/>
+      <c r="AA14" s="43"/>
+      <c r="AB14" s="43"/>
+      <c r="AC14" s="43"/>
+      <c r="AD14" s="43"/>
+      <c r="AE14" s="43"/>
+      <c r="AF14" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="AG14" s="57"/>
-      <c r="AH14" s="57"/>
-      <c r="AI14" s="58"/>
+      <c r="AG14" s="43"/>
+      <c r="AH14" s="43"/>
+      <c r="AI14" s="44"/>
       <c r="AJ14" s="28"/>
       <c r="AK14" s="5"/>
       <c r="AL14" s="5"/>
@@ -2384,43 +2403,43 @@
       <c r="AN14" s="5"/>
     </row>
     <row r="15" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="70">
+      <c r="B15" s="50">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="74"/>
-      <c r="O15" s="74"/>
-      <c r="P15" s="74"/>
-      <c r="Q15" s="75"/>
-      <c r="R15" s="75"/>
-      <c r="S15" s="75"/>
-      <c r="T15" s="66"/>
-      <c r="U15" s="66"/>
-      <c r="V15" s="66"/>
-      <c r="W15" s="66"/>
-      <c r="X15" s="66"/>
-      <c r="Y15" s="66"/>
-      <c r="Z15" s="66"/>
-      <c r="AA15" s="66"/>
-      <c r="AB15" s="66"/>
-      <c r="AC15" s="66"/>
-      <c r="AD15" s="66"/>
-      <c r="AE15" s="66"/>
-      <c r="AF15" s="67"/>
-      <c r="AG15" s="68"/>
-      <c r="AH15" s="68"/>
-      <c r="AI15" s="69"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="55"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="56"/>
+      <c r="V15" s="56"/>
+      <c r="W15" s="56"/>
+      <c r="X15" s="56"/>
+      <c r="Y15" s="56"/>
+      <c r="Z15" s="56"/>
+      <c r="AA15" s="56"/>
+      <c r="AB15" s="56"/>
+      <c r="AC15" s="56"/>
+      <c r="AD15" s="56"/>
+      <c r="AE15" s="56"/>
+      <c r="AF15" s="57"/>
+      <c r="AG15" s="58"/>
+      <c r="AH15" s="58"/>
+      <c r="AI15" s="59"/>
       <c r="AJ15" s="28"/>
       <c r="AK15" s="5"/>
       <c r="AL15" s="5"/>
@@ -2434,33 +2453,44 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="AF10:AI10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="W10:Z10"/>
-    <mergeCell ref="AA10:AE10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="T15:V15"/>
-    <mergeCell ref="W15:Z15"/>
-    <mergeCell ref="AA15:AE15"/>
-    <mergeCell ref="AF15:AI15"/>
-    <mergeCell ref="AA13:AE13"/>
-    <mergeCell ref="AF13:AI13"/>
-    <mergeCell ref="T14:V14"/>
-    <mergeCell ref="W14:Z14"/>
-    <mergeCell ref="AA14:AE14"/>
-    <mergeCell ref="AF14:AI14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="H14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="E2:Q2"/>
+    <mergeCell ref="T2:AF2"/>
+    <mergeCell ref="E3:Q3"/>
+    <mergeCell ref="T3:AF3"/>
+    <mergeCell ref="E4:Q4"/>
+    <mergeCell ref="T4:AF4"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="E5:Q5"/>
+    <mergeCell ref="T5:AF5"/>
+    <mergeCell ref="B7:N7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="W8:Z8"/>
+    <mergeCell ref="AA8:AE8"/>
+    <mergeCell ref="AF8:AI8"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="W9:Z9"/>
+    <mergeCell ref="AA9:AE9"/>
+    <mergeCell ref="AF9:AI9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="W11:Z11"/>
+    <mergeCell ref="AA11:AE11"/>
+    <mergeCell ref="AF11:AI11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:M10"/>
     <mergeCell ref="W12:Z12"/>
     <mergeCell ref="AA12:AE12"/>
     <mergeCell ref="AF12:AI12"/>
@@ -2477,48 +2507,37 @@
     <mergeCell ref="N12:P12"/>
     <mergeCell ref="Q12:S12"/>
     <mergeCell ref="T12:V12"/>
-    <mergeCell ref="AA9:AE9"/>
-    <mergeCell ref="AF9:AI9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="T11:V11"/>
-    <mergeCell ref="W11:Z11"/>
-    <mergeCell ref="AA11:AE11"/>
-    <mergeCell ref="AF11:AI11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="E5:Q5"/>
-    <mergeCell ref="T5:AF5"/>
-    <mergeCell ref="B7:N7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="W8:Z8"/>
-    <mergeCell ref="AA8:AE8"/>
-    <mergeCell ref="AF8:AI8"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="W9:Z9"/>
-    <mergeCell ref="E2:Q2"/>
-    <mergeCell ref="T2:AF2"/>
-    <mergeCell ref="E3:Q3"/>
-    <mergeCell ref="T3:AF3"/>
-    <mergeCell ref="E4:Q4"/>
-    <mergeCell ref="T4:AF4"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="H14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="T15:V15"/>
+    <mergeCell ref="W15:Z15"/>
+    <mergeCell ref="AA15:AE15"/>
+    <mergeCell ref="AF15:AI15"/>
+    <mergeCell ref="AA13:AE13"/>
+    <mergeCell ref="AF13:AI13"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="W14:Z14"/>
+    <mergeCell ref="AA14:AE14"/>
+    <mergeCell ref="AF14:AI14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="AF10:AI10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="W10:Z10"/>
+    <mergeCell ref="AA10:AE10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T9:V15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T9:V15" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"○,"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2532,7 +2551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -2561,38 +2580,38 @@
       <c r="F1" s="22"/>
     </row>
     <row r="2" spans="2:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
       <c r="R2" s="8"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="43" t="s">
+      <c r="T2" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="43"/>
-      <c r="AF2" s="43"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="74"/>
+      <c r="AA2" s="74"/>
+      <c r="AB2" s="74"/>
+      <c r="AC2" s="74"/>
+      <c r="AD2" s="74"/>
+      <c r="AE2" s="74"/>
+      <c r="AF2" s="74"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
@@ -2602,38 +2621,38 @@
       <c r="AM2" s="6"/>
     </row>
     <row r="3" spans="2:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="75"/>
       <c r="R3" s="9"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="44" t="s">
+      <c r="T3" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
-      <c r="W3" s="44"/>
-      <c r="X3" s="44"/>
-      <c r="Y3" s="44"/>
-      <c r="Z3" s="44"/>
-      <c r="AA3" s="44"/>
-      <c r="AB3" s="44"/>
-      <c r="AC3" s="44"/>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
+      <c r="U3" s="75"/>
+      <c r="V3" s="75"/>
+      <c r="W3" s="75"/>
+      <c r="X3" s="75"/>
+      <c r="Y3" s="75"/>
+      <c r="Z3" s="75"/>
+      <c r="AA3" s="75"/>
+      <c r="AB3" s="75"/>
+      <c r="AC3" s="75"/>
+      <c r="AD3" s="75"/>
+      <c r="AE3" s="75"/>
+      <c r="AF3" s="75"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
@@ -2642,36 +2661,36 @@
       <c r="AL3" s="1"/>
     </row>
     <row r="4" spans="2:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="43"/>
-      <c r="AE4" s="43"/>
-      <c r="AF4" s="43"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="74"/>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="74"/>
+      <c r="AE4" s="74"/>
+      <c r="AF4" s="74"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
@@ -2681,36 +2700,36 @@
       <c r="AM4" s="6"/>
     </row>
     <row r="5" spans="2:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="47"/>
-      <c r="U5" s="47"/>
-      <c r="V5" s="47"/>
-      <c r="W5" s="47"/>
-      <c r="X5" s="47"/>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="47"/>
-      <c r="AA5" s="47"/>
-      <c r="AB5" s="47"/>
-      <c r="AC5" s="47"/>
-      <c r="AD5" s="47"/>
-      <c r="AE5" s="47"/>
-      <c r="AF5" s="47"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="65"/>
+      <c r="Z5" s="65"/>
+      <c r="AA5" s="65"/>
+      <c r="AB5" s="65"/>
+      <c r="AC5" s="65"/>
+      <c r="AD5" s="65"/>
+      <c r="AE5" s="65"/>
+      <c r="AF5" s="65"/>
       <c r="AG5" s="7"/>
       <c r="AH5" s="7"/>
       <c r="AI5" s="7"/>
@@ -2734,21 +2753,21 @@
       <c r="O6" s="31"/>
     </row>
     <row r="7" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
       <c r="P7" s="26"/>
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
@@ -2776,58 +2795,58 @@
       <c r="AN7" s="3"/>
     </row>
     <row r="8" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52" t="s">
+      <c r="C8" s="69"/>
+      <c r="D8" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="53" t="s">
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="54" t="s">
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54" t="s">
+      <c r="O8" s="72"/>
+      <c r="P8" s="72"/>
+      <c r="Q8" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="R8" s="54"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54" t="s">
+      <c r="R8" s="72"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="U8" s="54"/>
-      <c r="V8" s="54"/>
-      <c r="W8" s="54" t="s">
+      <c r="U8" s="72"/>
+      <c r="V8" s="72"/>
+      <c r="W8" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="X8" s="54"/>
-      <c r="Y8" s="54"/>
-      <c r="Z8" s="54"/>
-      <c r="AA8" s="54" t="s">
+      <c r="X8" s="72"/>
+      <c r="Y8" s="72"/>
+      <c r="Z8" s="72"/>
+      <c r="AA8" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="AB8" s="54"/>
-      <c r="AC8" s="54"/>
-      <c r="AD8" s="54"/>
-      <c r="AE8" s="54"/>
-      <c r="AF8" s="54" t="s">
+      <c r="AB8" s="72"/>
+      <c r="AC8" s="72"/>
+      <c r="AD8" s="72"/>
+      <c r="AE8" s="72"/>
+      <c r="AF8" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="AG8" s="54"/>
-      <c r="AH8" s="54"/>
-      <c r="AI8" s="55"/>
+      <c r="AG8" s="72"/>
+      <c r="AH8" s="72"/>
+      <c r="AI8" s="73"/>
       <c r="AJ8" s="27"/>
       <c r="AK8" s="4"/>
       <c r="AL8" s="4"/>
@@ -2835,52 +2854,52 @@
       <c r="AN8" s="4"/>
     </row>
     <row r="9" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="59">
+      <c r="B9" s="45">
         <v>1</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="61" t="s">
+      <c r="C9" s="46"/>
+      <c r="D9" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="65" t="s">
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="45" t="s">
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="O9" s="45"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="56" t="s">
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="U9" s="56"/>
-      <c r="V9" s="57"/>
-      <c r="W9" s="76" t="s">
+      <c r="U9" s="49"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="X9" s="76"/>
-      <c r="Y9" s="76"/>
-      <c r="Z9" s="76"/>
-      <c r="AA9" s="57"/>
-      <c r="AB9" s="57"/>
-      <c r="AC9" s="57"/>
-      <c r="AD9" s="57"/>
-      <c r="AE9" s="57"/>
-      <c r="AF9" s="57"/>
-      <c r="AG9" s="57"/>
-      <c r="AH9" s="57"/>
-      <c r="AI9" s="58"/>
+      <c r="X9" s="77"/>
+      <c r="Y9" s="77"/>
+      <c r="Z9" s="77"/>
+      <c r="AA9" s="43"/>
+      <c r="AB9" s="43"/>
+      <c r="AC9" s="43"/>
+      <c r="AD9" s="43"/>
+      <c r="AE9" s="43"/>
+      <c r="AF9" s="43"/>
+      <c r="AG9" s="43"/>
+      <c r="AH9" s="43"/>
+      <c r="AI9" s="44"/>
       <c r="AJ9" s="28"/>
       <c r="AK9" s="5"/>
       <c r="AL9" s="5"/>
@@ -2888,54 +2907,54 @@
       <c r="AN9" s="5"/>
     </row>
     <row r="10" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="59">
+      <c r="B10" s="45">
         <v>2</v>
       </c>
-      <c r="C10" s="60">
+      <c r="C10" s="46">
         <v>2</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="65" t="s">
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
-      <c r="N10" s="45" t="s">
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="57" t="s">
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="U10" s="57"/>
-      <c r="V10" s="57"/>
-      <c r="W10" s="77"/>
-      <c r="X10" s="77"/>
-      <c r="Y10" s="77"/>
-      <c r="Z10" s="77"/>
-      <c r="AA10" s="57"/>
-      <c r="AB10" s="57"/>
-      <c r="AC10" s="57"/>
-      <c r="AD10" s="57"/>
-      <c r="AE10" s="57"/>
-      <c r="AF10" s="56" t="s">
+      <c r="U10" s="43"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="76"/>
+      <c r="X10" s="76"/>
+      <c r="Y10" s="76"/>
+      <c r="Z10" s="76"/>
+      <c r="AA10" s="43"/>
+      <c r="AB10" s="43"/>
+      <c r="AC10" s="43"/>
+      <c r="AD10" s="43"/>
+      <c r="AE10" s="43"/>
+      <c r="AF10" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="AG10" s="57"/>
-      <c r="AH10" s="57"/>
-      <c r="AI10" s="58"/>
+      <c r="AG10" s="43"/>
+      <c r="AH10" s="43"/>
+      <c r="AI10" s="44"/>
       <c r="AJ10" s="28"/>
       <c r="AK10" s="5"/>
       <c r="AL10" s="5"/>
@@ -2943,52 +2962,52 @@
       <c r="AN10" s="5"/>
     </row>
     <row r="11" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="59">
+      <c r="B11" s="45">
         <v>3</v>
       </c>
-      <c r="C11" s="60">
+      <c r="C11" s="46">
         <v>3</v>
       </c>
-      <c r="D11" s="61" t="s">
+      <c r="D11" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="65" t="s">
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="45" t="s">
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="O11" s="45"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="57" t="s">
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="U11" s="57"/>
-      <c r="V11" s="57"/>
-      <c r="W11" s="57"/>
-      <c r="X11" s="57"/>
-      <c r="Y11" s="57"/>
-      <c r="Z11" s="57"/>
-      <c r="AA11" s="57"/>
-      <c r="AB11" s="57"/>
-      <c r="AC11" s="57"/>
-      <c r="AD11" s="57"/>
-      <c r="AE11" s="57"/>
-      <c r="AF11" s="57"/>
-      <c r="AG11" s="57"/>
-      <c r="AH11" s="57"/>
-      <c r="AI11" s="58"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="43"/>
+      <c r="X11" s="43"/>
+      <c r="Y11" s="43"/>
+      <c r="Z11" s="43"/>
+      <c r="AA11" s="43"/>
+      <c r="AB11" s="43"/>
+      <c r="AC11" s="43"/>
+      <c r="AD11" s="43"/>
+      <c r="AE11" s="43"/>
+      <c r="AF11" s="43"/>
+      <c r="AG11" s="43"/>
+      <c r="AH11" s="43"/>
+      <c r="AI11" s="44"/>
       <c r="AJ11" s="28"/>
       <c r="AK11" s="5"/>
       <c r="AL11" s="5"/>
@@ -2996,48 +3015,48 @@
       <c r="AN11" s="5"/>
     </row>
     <row r="12" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="59">
+      <c r="B12" s="45">
         <v>4</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="61" t="s">
+      <c r="C12" s="46"/>
+      <c r="D12" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="65" t="s">
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="45" t="s">
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="57"/>
-      <c r="U12" s="57"/>
-      <c r="V12" s="57"/>
-      <c r="W12" s="57"/>
-      <c r="X12" s="57"/>
-      <c r="Y12" s="57"/>
-      <c r="Z12" s="57"/>
-      <c r="AA12" s="57"/>
-      <c r="AB12" s="57"/>
-      <c r="AC12" s="57"/>
-      <c r="AD12" s="57"/>
-      <c r="AE12" s="57"/>
-      <c r="AF12" s="57"/>
-      <c r="AG12" s="57"/>
-      <c r="AH12" s="57"/>
-      <c r="AI12" s="58"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43"/>
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="43"/>
+      <c r="AD12" s="43"/>
+      <c r="AE12" s="43"/>
+      <c r="AF12" s="43"/>
+      <c r="AG12" s="43"/>
+      <c r="AH12" s="43"/>
+      <c r="AI12" s="44"/>
       <c r="AJ12" s="28"/>
       <c r="AK12" s="5"/>
       <c r="AL12" s="5"/>
@@ -3045,48 +3064,48 @@
       <c r="AN12" s="5"/>
     </row>
     <row r="13" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="59">
+      <c r="B13" s="45">
         <v>5</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="61" t="s">
+      <c r="C13" s="46"/>
+      <c r="D13" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="65" t="s">
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="45" t="s">
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="61"/>
+      <c r="N13" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="46"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="57"/>
-      <c r="V13" s="57"/>
-      <c r="W13" s="57"/>
-      <c r="X13" s="57"/>
-      <c r="Y13" s="57"/>
-      <c r="Z13" s="57"/>
-      <c r="AA13" s="57"/>
-      <c r="AB13" s="57"/>
-      <c r="AC13" s="57"/>
-      <c r="AD13" s="57"/>
-      <c r="AE13" s="57"/>
-      <c r="AF13" s="57"/>
-      <c r="AG13" s="57"/>
-      <c r="AH13" s="57"/>
-      <c r="AI13" s="58"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="43"/>
+      <c r="U13" s="43"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="43"/>
+      <c r="X13" s="43"/>
+      <c r="Y13" s="43"/>
+      <c r="Z13" s="43"/>
+      <c r="AA13" s="43"/>
+      <c r="AB13" s="43"/>
+      <c r="AC13" s="43"/>
+      <c r="AD13" s="43"/>
+      <c r="AE13" s="43"/>
+      <c r="AF13" s="43"/>
+      <c r="AG13" s="43"/>
+      <c r="AH13" s="43"/>
+      <c r="AI13" s="44"/>
       <c r="AJ13" s="28"/>
       <c r="AK13" s="5"/>
       <c r="AL13" s="5"/>
@@ -3094,48 +3113,48 @@
       <c r="AN13" s="5"/>
     </row>
     <row r="14" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="59">
+      <c r="B14" s="45">
         <v>6</v>
       </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="61" t="s">
+      <c r="C14" s="46"/>
+      <c r="D14" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="65" t="s">
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="45" t="s">
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="O14" s="45"/>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="46"/>
-      <c r="S14" s="46"/>
-      <c r="T14" s="57"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="57"/>
-      <c r="W14" s="57"/>
-      <c r="X14" s="57"/>
-      <c r="Y14" s="57"/>
-      <c r="Z14" s="57"/>
-      <c r="AA14" s="57"/>
-      <c r="AB14" s="57"/>
-      <c r="AC14" s="57"/>
-      <c r="AD14" s="57"/>
-      <c r="AE14" s="57"/>
-      <c r="AF14" s="57"/>
-      <c r="AG14" s="57"/>
-      <c r="AH14" s="57"/>
-      <c r="AI14" s="58"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="43"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="43"/>
+      <c r="Y14" s="43"/>
+      <c r="Z14" s="43"/>
+      <c r="AA14" s="43"/>
+      <c r="AB14" s="43"/>
+      <c r="AC14" s="43"/>
+      <c r="AD14" s="43"/>
+      <c r="AE14" s="43"/>
+      <c r="AF14" s="43"/>
+      <c r="AG14" s="43"/>
+      <c r="AH14" s="43"/>
+      <c r="AI14" s="44"/>
       <c r="AJ14" s="28"/>
       <c r="AK14" s="5"/>
       <c r="AL14" s="5"/>
@@ -3143,54 +3162,54 @@
       <c r="AN14" s="5"/>
     </row>
     <row r="15" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="59">
+      <c r="B15" s="45">
         <v>7</v>
       </c>
-      <c r="C15" s="60"/>
-      <c r="D15" s="61" t="s">
+      <c r="C15" s="46"/>
+      <c r="D15" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="65" t="s">
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="45" t="s">
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="61"/>
+      <c r="N15" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="46">
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="48">
         <v>1</v>
       </c>
-      <c r="R15" s="46"/>
-      <c r="S15" s="46"/>
-      <c r="T15" s="57" t="s">
+      <c r="R15" s="48"/>
+      <c r="S15" s="48"/>
+      <c r="T15" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="57"/>
-      <c r="V15" s="57"/>
-      <c r="W15" s="57"/>
-      <c r="X15" s="57"/>
-      <c r="Y15" s="57"/>
-      <c r="Z15" s="57"/>
-      <c r="AA15" s="57"/>
-      <c r="AB15" s="57"/>
-      <c r="AC15" s="57"/>
-      <c r="AD15" s="57"/>
-      <c r="AE15" s="57"/>
-      <c r="AF15" s="56" t="s">
+      <c r="U15" s="43"/>
+      <c r="V15" s="43"/>
+      <c r="W15" s="43"/>
+      <c r="X15" s="43"/>
+      <c r="Y15" s="43"/>
+      <c r="Z15" s="43"/>
+      <c r="AA15" s="43"/>
+      <c r="AB15" s="43"/>
+      <c r="AC15" s="43"/>
+      <c r="AD15" s="43"/>
+      <c r="AE15" s="43"/>
+      <c r="AF15" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="AG15" s="57"/>
-      <c r="AH15" s="57"/>
-      <c r="AI15" s="58"/>
+      <c r="AG15" s="43"/>
+      <c r="AH15" s="43"/>
+      <c r="AI15" s="44"/>
       <c r="AJ15" s="28"/>
       <c r="AK15" s="5"/>
       <c r="AL15" s="5"/>
@@ -3198,44 +3217,44 @@
       <c r="AN15" s="5"/>
     </row>
     <row r="16" spans="2:40" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="70">
+      <c r="B16" s="50">
         <v>8</v>
       </c>
-      <c r="C16" s="71">
+      <c r="C16" s="51">
         <v>6</v>
       </c>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="74"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74"/>
-      <c r="Q16" s="75"/>
-      <c r="R16" s="75"/>
-      <c r="S16" s="75"/>
-      <c r="T16" s="66"/>
-      <c r="U16" s="66"/>
-      <c r="V16" s="66"/>
-      <c r="W16" s="66"/>
-      <c r="X16" s="66"/>
-      <c r="Y16" s="66"/>
-      <c r="Z16" s="66"/>
-      <c r="AA16" s="66"/>
-      <c r="AB16" s="66"/>
-      <c r="AC16" s="66"/>
-      <c r="AD16" s="66"/>
-      <c r="AE16" s="66"/>
-      <c r="AF16" s="67"/>
-      <c r="AG16" s="68"/>
-      <c r="AH16" s="68"/>
-      <c r="AI16" s="69"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="55"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56"/>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="56"/>
+      <c r="Z16" s="56"/>
+      <c r="AA16" s="56"/>
+      <c r="AB16" s="56"/>
+      <c r="AC16" s="56"/>
+      <c r="AD16" s="56"/>
+      <c r="AE16" s="56"/>
+      <c r="AF16" s="57"/>
+      <c r="AG16" s="58"/>
+      <c r="AH16" s="58"/>
+      <c r="AI16" s="59"/>
       <c r="AJ16" s="28"/>
       <c r="AK16" s="5"/>
       <c r="AL16" s="5"/>
@@ -3249,44 +3268,42 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="T14:V14"/>
-    <mergeCell ref="W14:Z14"/>
-    <mergeCell ref="AA14:AE14"/>
-    <mergeCell ref="AF14:AI14"/>
-    <mergeCell ref="T16:V16"/>
-    <mergeCell ref="W16:Z16"/>
-    <mergeCell ref="T15:V15"/>
-    <mergeCell ref="AA16:AE16"/>
-    <mergeCell ref="AF16:AI16"/>
-    <mergeCell ref="W15:Z15"/>
-    <mergeCell ref="AA15:AE15"/>
-    <mergeCell ref="AF15:AI15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="H14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="AA12:AE12"/>
-    <mergeCell ref="AF12:AI12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="T13:V13"/>
-    <mergeCell ref="W13:Z13"/>
-    <mergeCell ref="AA13:AE13"/>
-    <mergeCell ref="AF13:AI13"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="W9:Z9"/>
+    <mergeCell ref="E2:Q2"/>
+    <mergeCell ref="T2:AF2"/>
+    <mergeCell ref="E3:Q3"/>
+    <mergeCell ref="T3:AF3"/>
+    <mergeCell ref="E4:Q4"/>
+    <mergeCell ref="T4:AF4"/>
+    <mergeCell ref="E5:Q5"/>
+    <mergeCell ref="T5:AF5"/>
+    <mergeCell ref="B7:N7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="W8:Z8"/>
+    <mergeCell ref="AA8:AE8"/>
+    <mergeCell ref="AF8:AI8"/>
+    <mergeCell ref="AA9:AE9"/>
+    <mergeCell ref="AF9:AI9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="W10:Z10"/>
+    <mergeCell ref="AA10:AE10"/>
+    <mergeCell ref="AF10:AI10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q9:S9"/>
     <mergeCell ref="W11:Z11"/>
     <mergeCell ref="AA11:AE11"/>
     <mergeCell ref="AF11:AI11"/>
@@ -3303,46 +3320,48 @@
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="T11:V11"/>
-    <mergeCell ref="AA9:AE9"/>
-    <mergeCell ref="AF9:AI9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="W10:Z10"/>
-    <mergeCell ref="AA10:AE10"/>
-    <mergeCell ref="AF10:AI10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="E5:Q5"/>
-    <mergeCell ref="T5:AF5"/>
-    <mergeCell ref="B7:N7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="W8:Z8"/>
-    <mergeCell ref="AA8:AE8"/>
-    <mergeCell ref="AF8:AI8"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="W9:Z9"/>
-    <mergeCell ref="E2:Q2"/>
-    <mergeCell ref="T2:AF2"/>
-    <mergeCell ref="E3:Q3"/>
-    <mergeCell ref="T3:AF3"/>
-    <mergeCell ref="E4:Q4"/>
-    <mergeCell ref="T4:AF4"/>
+    <mergeCell ref="AA12:AE12"/>
+    <mergeCell ref="AF12:AI12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="W13:Z13"/>
+    <mergeCell ref="AA13:AE13"/>
+    <mergeCell ref="AF13:AI13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="H14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="W14:Z14"/>
+    <mergeCell ref="AA14:AE14"/>
+    <mergeCell ref="AF14:AI14"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="W16:Z16"/>
+    <mergeCell ref="T15:V15"/>
+    <mergeCell ref="AA16:AE16"/>
+    <mergeCell ref="AF16:AI16"/>
+    <mergeCell ref="W15:Z15"/>
+    <mergeCell ref="AA15:AE15"/>
+    <mergeCell ref="AF15:AI15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="Q16:S16"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T9:V16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T9:V16" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"○,"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>